<commit_message>
add: fix excel issue
</commit_message>
<xml_diff>
--- a/data/intent_emotion_mapping.xlsx
+++ b/data/intent_emotion_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dingdongliu/Desktop/Research/Grace_Robot/develop_stages/Grace_DM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F570BF5-F495-4590-BF82-99BBC76BB5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2587EE9-5C3C-7249-8848-363900B9E580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>(Q1.Skip) Age - Reach max limit</t>
   </si>
   <si>
-    <t xml:space="preserve">(Q1.Success) Age </t>
-  </si>
-  <si>
     <t>(Q2.Fail) Time - Doesn't know</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>(Q10.Success) Repeat Address</t>
+  </si>
+  <si>
+    <t>(Q1.Success) Age</t>
   </si>
 </sst>
 </file>
@@ -585,17 +585,17 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="45.6328125" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="5" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="5" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -717,7 +717,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -745,7 +745,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -773,7 +773,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -801,7 +801,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -829,7 +829,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -857,12 +857,12 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>
@@ -885,12 +885,12 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>23</v>
@@ -913,12 +913,12 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>26</v>
@@ -941,12 +941,12 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>28</v>
@@ -969,12 +969,12 @@
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
@@ -997,12 +997,12 @@
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>13</v>
@@ -1025,12 +1025,12 @@
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>23</v>
@@ -1053,12 +1053,12 @@
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>26</v>
@@ -1081,12 +1081,12 @@
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
         <v>16</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>28</v>
@@ -1109,12 +1109,12 @@
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>13</v>
@@ -1137,12 +1137,12 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>13</v>
@@ -1165,12 +1165,12 @@
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>23</v>
@@ -1193,12 +1193,12 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>26</v>
@@ -1221,12 +1221,12 @@
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
         <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>28</v>
@@ -1249,12 +1249,12 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8">
         <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>13</v>
@@ -1277,12 +1277,12 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8">
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>13</v>
@@ -1305,12 +1305,12 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8">
         <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>23</v>
@@ -1333,12 +1333,12 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8">
         <v>25</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>26</v>
@@ -1361,12 +1361,12 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="8">
         <v>26</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>28</v>
@@ -1389,12 +1389,12 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="8">
         <v>27</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>13</v>
@@ -1417,12 +1417,12 @@
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="8">
         <v>28</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>13</v>
@@ -1445,12 +1445,12 @@
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="8">
         <v>29</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>23</v>
@@ -1473,12 +1473,12 @@
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="8">
         <v>30</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>26</v>
@@ -1501,12 +1501,12 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="8">
         <v>31</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>28</v>
@@ -1529,12 +1529,12 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="8">
         <v>32</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>13</v>
@@ -1557,12 +1557,12 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="8">
         <v>33</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>13</v>
@@ -1585,12 +1585,12 @@
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="8">
         <v>34</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>23</v>
@@ -1613,12 +1613,12 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="8">
         <v>35</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>26</v>
@@ -1641,12 +1641,12 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>36</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>28</v>
@@ -1669,12 +1669,12 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="8">
         <v>37</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>13</v>
@@ -1697,12 +1697,12 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="8">
         <v>38</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>13</v>
@@ -1725,12 +1725,12 @@
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="8">
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>23</v>
@@ -1753,12 +1753,12 @@
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="8">
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>26</v>
@@ -1781,12 +1781,12 @@
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="8">
         <v>41</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>28</v>
@@ -1809,12 +1809,12 @@
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="8">
         <v>42</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>13</v>
@@ -1837,12 +1837,12 @@
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="8">
         <v>43</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>13</v>
@@ -1865,12 +1865,12 @@
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="8">
         <v>44</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>23</v>
@@ -1893,12 +1893,12 @@
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="8">
         <v>45</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>26</v>
@@ -1921,12 +1921,12 @@
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="8">
         <v>46</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>28</v>
@@ -1949,12 +1949,12 @@
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="8">
         <v>47</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>13</v>
@@ -1977,12 +1977,12 @@
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="8">
         <v>48</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>13</v>
@@ -2005,12 +2005,12 @@
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="8">
         <v>49</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>23</v>
@@ -2033,12 +2033,12 @@
       <c r="K51" s="7"/>
       <c r="L51" s="7"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="8">
         <v>50</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>26</v>
@@ -2061,12 +2061,12 @@
       <c r="K52" s="7"/>
       <c r="L52" s="7"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="8">
         <v>51</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>28</v>
@@ -2089,12 +2089,12 @@
       <c r="K53" s="7"/>
       <c r="L53" s="7"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="8">
         <v>52</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>13</v>
@@ -2117,12 +2117,12 @@
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" s="8">
         <v>53</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>13</v>
@@ -2145,12 +2145,12 @@
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="8">
         <v>54</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>23</v>
@@ -2173,12 +2173,12 @@
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" s="8">
         <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>26</v>
@@ -2201,12 +2201,12 @@
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="8">
         <v>56</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>28</v>
@@ -2229,12 +2229,12 @@
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="8">
         <v>57</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>13</v>
@@ -2257,12 +2257,12 @@
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" s="8">
         <v>58</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Fixing intent emotion mapping age success
</commit_message>
<xml_diff>
--- a/data/intent_emotion_mapping.xlsx
+++ b/data/intent_emotion_mapping.xlsx
@@ -106,7 +106,7 @@
     <t>(Q1.Skip) Age - Reach max limit</t>
   </si>
   <si>
-    <t xml:space="preserve">(Q1.Success) Age </t>
+    <t>(Q1.Success) Age</t>
   </si>
   <si>
     <t>(Q2.Fail) Time - Doesn't know</t>
@@ -337,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -361,6 +361,9 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -859,7 +862,7 @@
       <c r="A10" s="2">
         <v>8.0</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -884,10 +887,10 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>9.0</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -912,10 +915,10 @@
       <c r="L11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>10.0</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -940,10 +943,10 @@
       <c r="L12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>11.0</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -968,10 +971,10 @@
       <c r="L13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>12.0</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -996,10 +999,10 @@
       <c r="L14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>13.0</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1024,10 +1027,10 @@
       <c r="L15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>14.0</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1052,10 +1055,10 @@
       <c r="L16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="8">
+      <c r="A17" s="9">
         <v>15.0</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1080,10 +1083,10 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="8">
+      <c r="A18" s="9">
         <v>16.0</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1108,10 +1111,10 @@
       <c r="L18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="8">
+      <c r="A19" s="9">
         <v>17.0</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -1136,10 +1139,10 @@
       <c r="L19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="8">
+      <c r="A20" s="9">
         <v>18.0</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1164,10 +1167,10 @@
       <c r="L20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="8">
+      <c r="A21" s="9">
         <v>19.0</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1192,10 +1195,10 @@
       <c r="L21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>20.0</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1220,10 +1223,10 @@
       <c r="L22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="8">
+      <c r="A23" s="9">
         <v>21.0</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1248,10 +1251,10 @@
       <c r="L23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="8">
+      <c r="A24" s="9">
         <v>22.0</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="6" t="s">
@@ -1276,10 +1279,10 @@
       <c r="L24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="8">
+      <c r="A25" s="9">
         <v>23.0</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1304,10 +1307,10 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="8">
+      <c r="A26" s="9">
         <v>24.0</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1332,10 +1335,10 @@
       <c r="L26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="8">
+      <c r="A27" s="9">
         <v>25.0</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1360,10 +1363,10 @@
       <c r="L27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="8">
+      <c r="A28" s="9">
         <v>26.0</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="6" t="s">
@@ -1388,10 +1391,10 @@
       <c r="L28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="8">
+      <c r="A29" s="9">
         <v>27.0</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="6" t="s">
@@ -1416,10 +1419,10 @@
       <c r="L29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="8">
+      <c r="A30" s="9">
         <v>28.0</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="6" t="s">
@@ -1444,10 +1447,10 @@
       <c r="L30" s="7"/>
     </row>
     <row r="31">
-      <c r="A31" s="8">
+      <c r="A31" s="9">
         <v>29.0</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="6" t="s">
@@ -1472,10 +1475,10 @@
       <c r="L31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="8">
+      <c r="A32" s="9">
         <v>30.0</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -1500,10 +1503,10 @@
       <c r="L32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="8">
+      <c r="A33" s="9">
         <v>31.0</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="6" t="s">
@@ -1528,10 +1531,10 @@
       <c r="L33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="8">
+      <c r="A34" s="9">
         <v>32.0</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -1556,10 +1559,10 @@
       <c r="L34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="8">
+      <c r="A35" s="9">
         <v>33.0</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1584,10 +1587,10 @@
       <c r="L35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="8">
+      <c r="A36" s="9">
         <v>34.0</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>57</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -1612,10 +1615,10 @@
       <c r="L36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="8">
+      <c r="A37" s="9">
         <v>35.0</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -1640,10 +1643,10 @@
       <c r="L37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="8">
+      <c r="A38" s="9">
         <v>36.0</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="6" t="s">
@@ -1668,10 +1671,10 @@
       <c r="L38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="8">
+      <c r="A39" s="9">
         <v>37.0</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -1696,10 +1699,10 @@
       <c r="L39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="8">
+      <c r="A40" s="9">
         <v>38.0</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C40" s="6" t="s">
@@ -1724,10 +1727,10 @@
       <c r="L40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="8">
+      <c r="A41" s="9">
         <v>39.0</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -1752,10 +1755,10 @@
       <c r="L41" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="8">
+      <c r="A42" s="9">
         <v>40.0</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C42" s="6" t="s">
@@ -1780,10 +1783,10 @@
       <c r="L42" s="7"/>
     </row>
     <row r="43">
-      <c r="A43" s="8">
+      <c r="A43" s="9">
         <v>41.0</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C43" s="6" t="s">
@@ -1808,10 +1811,10 @@
       <c r="L43" s="7"/>
     </row>
     <row r="44">
-      <c r="A44" s="8">
+      <c r="A44" s="9">
         <v>42.0</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C44" s="6" t="s">
@@ -1836,10 +1839,10 @@
       <c r="L44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="8">
+      <c r="A45" s="9">
         <v>43.0</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C45" s="6" t="s">
@@ -1864,10 +1867,10 @@
       <c r="L45" s="7"/>
     </row>
     <row r="46">
-      <c r="A46" s="8">
+      <c r="A46" s="9">
         <v>44.0</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C46" s="6" t="s">
@@ -1892,10 +1895,10 @@
       <c r="L46" s="7"/>
     </row>
     <row r="47">
-      <c r="A47" s="8">
+      <c r="A47" s="9">
         <v>45.0</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C47" s="6" t="s">
@@ -1920,10 +1923,10 @@
       <c r="L47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="8">
+      <c r="A48" s="9">
         <v>46.0</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -1948,10 +1951,10 @@
       <c r="L48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="8">
+      <c r="A49" s="9">
         <v>47.0</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="6" t="s">
@@ -1976,10 +1979,10 @@
       <c r="L49" s="7"/>
     </row>
     <row r="50">
-      <c r="A50" s="8">
+      <c r="A50" s="9">
         <v>48.0</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C50" s="6" t="s">
@@ -2004,10 +2007,10 @@
       <c r="L50" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="8">
+      <c r="A51" s="9">
         <v>49.0</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>72</v>
       </c>
       <c r="C51" s="6" t="s">
@@ -2032,10 +2035,10 @@
       <c r="L51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="8">
+      <c r="A52" s="9">
         <v>50.0</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C52" s="6" t="s">
@@ -2060,10 +2063,10 @@
       <c r="L52" s="7"/>
     </row>
     <row r="53">
-      <c r="A53" s="8">
+      <c r="A53" s="9">
         <v>51.0</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="10" t="s">
         <v>74</v>
       </c>
       <c r="C53" s="6" t="s">
@@ -2088,10 +2091,10 @@
       <c r="L53" s="7"/>
     </row>
     <row r="54">
-      <c r="A54" s="8">
+      <c r="A54" s="9">
         <v>52.0</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="10" t="s">
         <v>75</v>
       </c>
       <c r="C54" s="6" t="s">
@@ -2116,10 +2119,10 @@
       <c r="L54" s="7"/>
     </row>
     <row r="55">
-      <c r="A55" s="8">
+      <c r="A55" s="9">
         <v>53.0</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C55" s="6" t="s">
@@ -2144,10 +2147,10 @@
       <c r="L55" s="7"/>
     </row>
     <row r="56">
-      <c r="A56" s="8">
+      <c r="A56" s="9">
         <v>54.0</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C56" s="6" t="s">
@@ -2172,10 +2175,10 @@
       <c r="L56" s="7"/>
     </row>
     <row r="57">
-      <c r="A57" s="8">
+      <c r="A57" s="9">
         <v>55.0</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="10" t="s">
         <v>78</v>
       </c>
       <c r="C57" s="6" t="s">
@@ -2200,10 +2203,10 @@
       <c r="L57" s="7"/>
     </row>
     <row r="58">
-      <c r="A58" s="8">
+      <c r="A58" s="9">
         <v>56.0</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C58" s="6" t="s">
@@ -2228,10 +2231,10 @@
       <c r="L58" s="7"/>
     </row>
     <row r="59">
-      <c r="A59" s="8">
+      <c r="A59" s="9">
         <v>57.0</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="10" t="s">
         <v>80</v>
       </c>
       <c r="C59" s="6" t="s">
@@ -2256,10 +2259,10 @@
       <c r="L59" s="7"/>
     </row>
     <row r="60">
-      <c r="A60" s="8">
+      <c r="A60" s="9">
         <v>58.0</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C60" s="6" t="s">
@@ -2284,10 +2287,10 @@
       <c r="L60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="8">
+      <c r="A61" s="9">
         <v>59.0</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="11" t="s">
         <v>82</v>
       </c>
       <c r="C61" s="6" t="s">
@@ -2305,17 +2308,17 @@
       <c r="G61" s="6">
         <v>80.0</v>
       </c>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
     </row>
     <row r="62">
-      <c r="A62" s="8">
+      <c r="A62" s="9">
         <v>60.0</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="11" t="s">
         <v>83</v>
       </c>
       <c r="C62" s="6" t="s">
@@ -2333,17 +2336,17 @@
       <c r="G62" s="6">
         <v>80.0</v>
       </c>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
     </row>
     <row r="63">
-      <c r="A63" s="8">
+      <c r="A63" s="9">
         <v>61.0</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C63" s="6" t="s">
@@ -2361,11 +2364,11 @@
       <c r="G63" s="6">
         <v>80.0</v>
       </c>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+      <c r="L63" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Tuned windows a bit
</commit_message>
<xml_diff>
--- a/data/intent_emotion_mapping.xlsx
+++ b/data/intent_emotion_mapping.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="91">
   <si>
     <t>nb</t>
   </si>
@@ -25,7 +25,7 @@
     <t>POSES</t>
   </si>
   <si>
-    <t>Magnitude</t>
+    <t>E_Magnitude</t>
   </si>
   <si>
     <t>E_Start (%)</t>
@@ -34,19 +34,16 @@
     <t>E_End (%)</t>
   </si>
   <si>
-    <t>E_Para</t>
-  </si>
-  <si>
-    <t>Gestures</t>
-  </si>
-  <si>
-    <t>G_Start</t>
-  </si>
-  <si>
-    <t>G_End</t>
-  </si>
-  <si>
-    <t>G_Para</t>
+    <t>GESTURES</t>
+  </si>
+  <si>
+    <t>G_Start (%)</t>
+  </si>
+  <si>
+    <t>G_End (%)</t>
+  </si>
+  <si>
+    <t>G_Magnitude</t>
   </si>
   <si>
     <t>Default Welcome Intent</t>
@@ -58,6 +55,9 @@
     <t>happy</t>
   </si>
   <si>
+    <t>MAIN-2</t>
+  </si>
+  <si>
     <t>(Q0.Fail) How are you - From fallback</t>
   </si>
   <si>
@@ -67,6 +67,9 @@
     <t>engaged</t>
   </si>
   <si>
+    <t>MAIN-SIT_1-B_Smallandbig</t>
+  </si>
+  <si>
     <t>(Q0.Success) How are you - Bad</t>
   </si>
   <si>
@@ -76,9 +79,15 @@
     <t>worry</t>
   </si>
   <si>
+    <t>MAIN-1</t>
+  </si>
+  <si>
     <t>(Q0.Success) How are you - Good</t>
   </si>
   <si>
+    <t>MAIN-SIT_1-R_Likesth</t>
+  </si>
+  <si>
     <t>(Q1.Fail) Age - Doesn't know</t>
   </si>
   <si>
@@ -88,6 +97,9 @@
     <t>recoil</t>
   </si>
   <si>
+    <t>MAIN-OOPS</t>
+  </si>
+  <si>
     <t>(Q1.Fail) Age - From fallback</t>
   </si>
   <si>
@@ -106,6 +118,9 @@
     <t>(Q1.Skip) Age - Reach max limit</t>
   </si>
   <si>
+    <t>MAIN-SIT_1-R_Thanksfor3</t>
+  </si>
+  <si>
     <t>(Q1.Success) Age</t>
   </si>
   <si>
@@ -257,6 +272,9 @@
   </si>
   <si>
     <t>(Q10.Success) Repeat Address</t>
+  </si>
+  <si>
+    <t>MAIN-SIT_0-R_bye</t>
   </si>
   <si>
     <t>(Special) Gracefully exit</t>
@@ -360,7 +378,10 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -374,7 +395,6 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -594,6 +614,7 @@
     <col customWidth="1" min="2" max="2" width="45.63"/>
     <col customWidth="1" min="3" max="3" width="17.38"/>
     <col customWidth="1" min="4" max="5" width="17.63"/>
+    <col customWidth="1" min="8" max="8" width="43.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -630,22 +651,19 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>0.0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="5">
         <v>0.85</v>
@@ -656,11 +674,18 @@
       <c r="G2" s="6">
         <v>80.0</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -684,24 +709,31 @@
       <c r="G3" s="6">
         <v>80.0</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
         <v>2.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5">
         <v>0.6</v>
@@ -712,24 +744,31 @@
       <c r="G4" s="6">
         <v>80.0</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
         <v>3.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="E5" s="5">
         <v>0.85</v>
@@ -740,24 +779,31 @@
       <c r="G5" s="6">
         <v>80.0</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
         <v>4.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5">
         <v>0.75</v>
@@ -768,21 +814,28 @@
       <c r="G6" s="6">
         <v>80.0</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>5.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>17</v>
@@ -796,24 +849,31 @@
       <c r="G7" s="6">
         <v>80.0</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J7" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>6.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" s="5">
         <v>0.75</v>
@@ -824,24 +884,31 @@
       <c r="G8" s="6">
         <v>80.0</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J8" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
         <v>7.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5">
         <v>0.65</v>
@@ -852,21 +919,28 @@
       <c r="G9" s="6">
         <v>80.0</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
         <v>8.0</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>31</v>
+      <c r="B10" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>17</v>
@@ -880,24 +954,31 @@
       <c r="G10" s="6">
         <v>80.0</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="9">
+      <c r="A11" s="10">
         <v>9.0</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>32</v>
+      <c r="B11" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="5">
         <v>0.75</v>
@@ -908,21 +989,28 @@
       <c r="G11" s="6">
         <v>80.0</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="9">
+      <c r="A12" s="10">
         <v>10.0</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>33</v>
+      <c r="B12" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>17</v>
@@ -936,24 +1024,31 @@
       <c r="G12" s="6">
         <v>80.0</v>
       </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="9">
+      <c r="A13" s="10">
         <v>11.0</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>34</v>
+      <c r="B13" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E13" s="5">
         <v>0.75</v>
@@ -964,24 +1059,31 @@
       <c r="G13" s="6">
         <v>80.0</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="9">
+      <c r="A14" s="10">
         <v>12.0</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>35</v>
+      <c r="B14" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="5">
         <v>0.65</v>
@@ -992,21 +1094,28 @@
       <c r="G14" s="6">
         <v>80.0</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J14" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="9">
+      <c r="A15" s="10">
         <v>13.0</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>17</v>
@@ -1020,24 +1129,31 @@
       <c r="G15" s="6">
         <v>80.0</v>
       </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="9">
+      <c r="A16" s="10">
         <v>14.0</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>37</v>
+      <c r="B16" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" s="5">
         <v>0.75</v>
@@ -1048,21 +1164,28 @@
       <c r="G16" s="6">
         <v>80.0</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J16" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="9">
+      <c r="A17" s="10">
         <v>15.0</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>38</v>
+      <c r="B17" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>17</v>
@@ -1076,24 +1199,31 @@
       <c r="G17" s="6">
         <v>80.0</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="9">
+      <c r="A18" s="10">
         <v>16.0</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>39</v>
+      <c r="B18" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5">
         <v>0.75</v>
@@ -1104,24 +1234,31 @@
       <c r="G18" s="6">
         <v>80.0</v>
       </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J18" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="9">
+      <c r="A19" s="10">
         <v>17.0</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>40</v>
+      <c r="B19" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E19" s="5">
         <v>0.65</v>
@@ -1132,21 +1269,28 @@
       <c r="G19" s="6">
         <v>80.0</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="9">
+      <c r="A20" s="10">
         <v>18.0</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>41</v>
+      <c r="B20" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>17</v>
@@ -1160,24 +1304,31 @@
       <c r="G20" s="6">
         <v>80.0</v>
       </c>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J20" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K20" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="9">
+      <c r="A21" s="10">
         <v>19.0</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>42</v>
+      <c r="B21" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E21" s="5">
         <v>0.75</v>
@@ -1188,21 +1339,28 @@
       <c r="G21" s="6">
         <v>80.0</v>
       </c>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J21" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="9">
+      <c r="A22" s="10">
         <v>20.0</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>43</v>
+      <c r="B22" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>17</v>
@@ -1216,24 +1374,31 @@
       <c r="G22" s="6">
         <v>80.0</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J22" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K22" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="9">
+      <c r="A23" s="10">
         <v>21.0</v>
       </c>
-      <c r="B23" s="10" t="s">
-        <v>44</v>
+      <c r="B23" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E23" s="5">
         <v>0.75</v>
@@ -1244,24 +1409,31 @@
       <c r="G23" s="6">
         <v>80.0</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J23" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K23" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="9">
+      <c r="A24" s="10">
         <v>22.0</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>45</v>
+      <c r="B24" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E24" s="5">
         <v>0.65</v>
@@ -1272,21 +1444,28 @@
       <c r="G24" s="6">
         <v>80.0</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J24" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="9">
+      <c r="A25" s="10">
         <v>23.0</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>46</v>
+      <c r="B25" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>17</v>
@@ -1300,24 +1479,31 @@
       <c r="G25" s="6">
         <v>80.0</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J25" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="9">
+      <c r="A26" s="10">
         <v>24.0</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>47</v>
+      <c r="B26" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E26" s="5">
         <v>0.75</v>
@@ -1328,21 +1514,28 @@
       <c r="G26" s="6">
         <v>80.0</v>
       </c>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K26" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="9">
+      <c r="A27" s="10">
         <v>25.0</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>48</v>
+      <c r="B27" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>17</v>
@@ -1356,24 +1549,31 @@
       <c r="G27" s="6">
         <v>80.0</v>
       </c>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="H27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J27" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K27" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="9">
+      <c r="A28" s="10">
         <v>26.0</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>49</v>
+      <c r="B28" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E28" s="5">
         <v>0.75</v>
@@ -1384,24 +1584,31 @@
       <c r="G28" s="6">
         <v>80.0</v>
       </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
+      <c r="H28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K28" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="9">
+      <c r="A29" s="10">
         <v>27.0</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>50</v>
+      <c r="B29" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E29" s="5">
         <v>0.65</v>
@@ -1412,21 +1619,28 @@
       <c r="G29" s="6">
         <v>80.0</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="H29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J29" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="9">
+      <c r="A30" s="10">
         <v>28.0</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>51</v>
+      <c r="B30" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>17</v>
@@ -1440,24 +1654,31 @@
       <c r="G30" s="6">
         <v>80.0</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
+      <c r="H30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J30" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="9">
+      <c r="A31" s="10">
         <v>29.0</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>52</v>
+      <c r="B31" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E31" s="5">
         <v>0.75</v>
@@ -1468,21 +1689,28 @@
       <c r="G31" s="6">
         <v>80.0</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
+      <c r="H31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J31" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="9">
+      <c r="A32" s="10">
         <v>30.0</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>53</v>
+      <c r="B32" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>17</v>
@@ -1496,24 +1724,31 @@
       <c r="G32" s="6">
         <v>80.0</v>
       </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
+      <c r="H32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I32" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J32" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K32" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="9">
+      <c r="A33" s="10">
         <v>31.0</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>54</v>
+      <c r="B33" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E33" s="5">
         <v>0.75</v>
@@ -1524,24 +1759,31 @@
       <c r="G33" s="6">
         <v>80.0</v>
       </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J33" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K33" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="9">
+      <c r="A34" s="10">
         <v>32.0</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>55</v>
+      <c r="B34" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E34" s="5">
         <v>0.65</v>
@@ -1552,21 +1794,28 @@
       <c r="G34" s="6">
         <v>80.0</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
+      <c r="H34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J34" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="9">
+      <c r="A35" s="10">
         <v>33.0</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>56</v>
+      <c r="B35" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>17</v>
@@ -1580,24 +1829,31 @@
       <c r="G35" s="6">
         <v>80.0</v>
       </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
+      <c r="H35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J35" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K35" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="9">
+      <c r="A36" s="10">
         <v>34.0</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>57</v>
+      <c r="B36" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E36" s="5">
         <v>0.75</v>
@@ -1608,21 +1864,28 @@
       <c r="G36" s="6">
         <v>80.0</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
+      <c r="H36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J36" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K36" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="9">
+      <c r="A37" s="10">
         <v>35.0</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>58</v>
+      <c r="B37" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>17</v>
@@ -1636,24 +1899,31 @@
       <c r="G37" s="6">
         <v>80.0</v>
       </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
+      <c r="H37" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J37" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K37" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="9">
+      <c r="A38" s="10">
         <v>36.0</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>59</v>
+      <c r="B38" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E38" s="5">
         <v>0.75</v>
@@ -1664,24 +1934,31 @@
       <c r="G38" s="6">
         <v>80.0</v>
       </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
+      <c r="H38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I38" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J38" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K38" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="9">
+      <c r="A39" s="10">
         <v>37.0</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>60</v>
+      <c r="B39" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E39" s="5">
         <v>0.65</v>
@@ -1692,21 +1969,28 @@
       <c r="G39" s="6">
         <v>80.0</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
+      <c r="H39" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I39" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J39" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K39" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="9">
+      <c r="A40" s="10">
         <v>38.0</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>61</v>
+      <c r="B40" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>17</v>
@@ -1720,24 +2004,31 @@
       <c r="G40" s="6">
         <v>80.0</v>
       </c>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J40" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="9">
+      <c r="A41" s="10">
         <v>39.0</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>62</v>
+      <c r="B41" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E41" s="5">
         <v>0.75</v>
@@ -1748,21 +2039,28 @@
       <c r="G41" s="6">
         <v>80.0</v>
       </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
+      <c r="H41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J41" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K41" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="9">
+      <c r="A42" s="10">
         <v>40.0</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>63</v>
+      <c r="B42" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>17</v>
@@ -1776,24 +2074,31 @@
       <c r="G42" s="6">
         <v>80.0</v>
       </c>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
+      <c r="H42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J42" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K42" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="9">
+      <c r="A43" s="10">
         <v>41.0</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>64</v>
+      <c r="B43" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E43" s="5">
         <v>0.75</v>
@@ -1804,24 +2109,31 @@
       <c r="G43" s="6">
         <v>80.0</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
+      <c r="H43" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J43" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K43" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="9">
+      <c r="A44" s="10">
         <v>42.0</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>65</v>
+      <c r="B44" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E44" s="5">
         <v>0.65</v>
@@ -1832,21 +2144,28 @@
       <c r="G44" s="6">
         <v>80.0</v>
       </c>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
+      <c r="H44" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I44" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J44" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K44" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="9">
+      <c r="A45" s="10">
         <v>43.0</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>66</v>
+      <c r="B45" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>17</v>
@@ -1860,24 +2179,31 @@
       <c r="G45" s="6">
         <v>80.0</v>
       </c>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
+      <c r="H45" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I45" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J45" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K45" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="9">
+      <c r="A46" s="10">
         <v>44.0</v>
       </c>
-      <c r="B46" s="10" t="s">
-        <v>67</v>
+      <c r="B46" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E46" s="5">
         <v>0.75</v>
@@ -1888,21 +2214,28 @@
       <c r="G46" s="6">
         <v>80.0</v>
       </c>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
+      <c r="H46" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J46" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K46" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="9">
+      <c r="A47" s="10">
         <v>45.0</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>68</v>
+      <c r="B47" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>17</v>
@@ -1916,24 +2249,31 @@
       <c r="G47" s="6">
         <v>80.0</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7"/>
+      <c r="H47" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J47" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K47" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="9">
+      <c r="A48" s="10">
         <v>46.0</v>
       </c>
-      <c r="B48" s="10" t="s">
-        <v>69</v>
+      <c r="B48" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E48" s="5">
         <v>0.75</v>
@@ -1944,24 +2284,31 @@
       <c r="G48" s="6">
         <v>80.0</v>
       </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7"/>
+      <c r="H48" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I48" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J48" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K48" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="9">
+      <c r="A49" s="10">
         <v>47.0</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>70</v>
+      <c r="B49" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E49" s="5">
         <v>0.65</v>
@@ -1972,21 +2319,28 @@
       <c r="G49" s="6">
         <v>80.0</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
+      <c r="H49" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J49" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K49" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="9">
+      <c r="A50" s="10">
         <v>48.0</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>71</v>
+      <c r="B50" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>17</v>
@@ -2000,24 +2354,31 @@
       <c r="G50" s="6">
         <v>80.0</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
+      <c r="H50" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I50" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J50" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K50" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="9">
+      <c r="A51" s="10">
         <v>49.0</v>
       </c>
-      <c r="B51" s="10" t="s">
-        <v>72</v>
+      <c r="B51" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E51" s="5">
         <v>0.75</v>
@@ -2028,21 +2389,28 @@
       <c r="G51" s="6">
         <v>80.0</v>
       </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
+      <c r="H51" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J51" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K51" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="9">
+      <c r="A52" s="10">
         <v>50.0</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>73</v>
+      <c r="B52" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>17</v>
@@ -2056,24 +2424,31 @@
       <c r="G52" s="6">
         <v>80.0</v>
       </c>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="7"/>
-      <c r="L52" s="7"/>
+      <c r="H52" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J52" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K52" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="9">
+      <c r="A53" s="10">
         <v>51.0</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>74</v>
+      <c r="B53" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E53" s="5">
         <v>0.75</v>
@@ -2084,24 +2459,31 @@
       <c r="G53" s="6">
         <v>80.0</v>
       </c>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
+      <c r="H53" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J53" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K53" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="9">
+      <c r="A54" s="10">
         <v>52.0</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>75</v>
+      <c r="B54" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E54" s="5">
         <v>0.65</v>
@@ -2112,21 +2494,28 @@
       <c r="G54" s="6">
         <v>80.0</v>
       </c>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
+      <c r="H54" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I54" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J54" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K54" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="9">
+      <c r="A55" s="10">
         <v>53.0</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>76</v>
+      <c r="B55" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>17</v>
@@ -2140,24 +2529,31 @@
       <c r="G55" s="6">
         <v>80.0</v>
       </c>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="7"/>
+      <c r="H55" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I55" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J55" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K55" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="9">
+      <c r="A56" s="10">
         <v>54.0</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>77</v>
+      <c r="B56" s="11" t="s">
+        <v>82</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E56" s="5">
         <v>0.75</v>
@@ -2168,21 +2564,28 @@
       <c r="G56" s="6">
         <v>80.0</v>
       </c>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
+      <c r="H56" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J56" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K56" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="9">
+      <c r="A57" s="10">
         <v>55.0</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>78</v>
+      <c r="B57" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>17</v>
@@ -2196,24 +2599,31 @@
       <c r="G57" s="6">
         <v>80.0</v>
       </c>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
+      <c r="H57" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J57" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K57" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="9">
+      <c r="A58" s="10">
         <v>56.0</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>79</v>
+      <c r="B58" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E58" s="5">
         <v>0.75</v>
@@ -2224,24 +2634,31 @@
       <c r="G58" s="6">
         <v>80.0</v>
       </c>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
+      <c r="H58" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I58" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J58" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K58" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="9">
+      <c r="A59" s="10">
         <v>57.0</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>80</v>
+      <c r="B59" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E59" s="5">
         <v>0.65</v>
@@ -2252,21 +2669,28 @@
       <c r="G59" s="6">
         <v>80.0</v>
       </c>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
+      <c r="H59" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J59" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K59" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="9">
+      <c r="A60" s="10">
         <v>58.0</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>81</v>
+      <c r="B60" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>17</v>
@@ -2280,24 +2704,31 @@
       <c r="G60" s="6">
         <v>80.0</v>
       </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
+      <c r="H60" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I60" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J60" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K60" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="9">
+      <c r="A61" s="10">
         <v>59.0</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>82</v>
+      <c r="B61" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E61" s="5">
         <v>0.65</v>
@@ -2308,21 +2739,28 @@
       <c r="G61" s="6">
         <v>80.0</v>
       </c>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="K61" s="12"/>
-      <c r="L61" s="12"/>
+      <c r="H61" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I61" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J61" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K61" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="9">
+      <c r="A62" s="10">
         <v>60.0</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>83</v>
+      <c r="B62" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>17</v>
@@ -2336,21 +2774,28 @@
       <c r="G62" s="6">
         <v>80.0</v>
       </c>
-      <c r="H62" s="12"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="K62" s="12"/>
-      <c r="L62" s="12"/>
+      <c r="H62" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I62" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J62" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K62" s="8">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="9">
+      <c r="A63" s="10">
         <v>61.0</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>84</v>
+      <c r="B63" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>17</v>
@@ -2364,11 +2809,18 @@
       <c r="G63" s="6">
         <v>80.0</v>
       </c>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
+      <c r="H63" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I63" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="J63" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="K63" s="8">
+        <v>1.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Commented bardging handling, updated dialogue flowdata base.
</commit_message>
<xml_diff>
--- a/data/intent_emotion_mapping.xlsx
+++ b/data/intent_emotion_mapping.xlsx
@@ -806,7 +806,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F6" s="6">
         <v>5.0</v>
@@ -911,7 +911,7 @@
         <v>27</v>
       </c>
       <c r="E9" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F9" s="6">
         <v>5.0</v>
@@ -981,7 +981,7 @@
         <v>27</v>
       </c>
       <c r="E11" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F11" s="6">
         <v>5.0</v>
@@ -1086,7 +1086,7 @@
         <v>27</v>
       </c>
       <c r="E14" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F14" s="6">
         <v>5.0</v>
@@ -1156,7 +1156,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F16" s="6">
         <v>5.0</v>
@@ -1261,7 +1261,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F19" s="6">
         <v>5.0</v>
@@ -1331,7 +1331,7 @@
         <v>27</v>
       </c>
       <c r="E21" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F21" s="6">
         <v>5.0</v>
@@ -1436,7 +1436,7 @@
         <v>27</v>
       </c>
       <c r="E24" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F24" s="6">
         <v>5.0</v>
@@ -1506,7 +1506,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F26" s="6">
         <v>5.0</v>
@@ -1611,7 +1611,7 @@
         <v>27</v>
       </c>
       <c r="E29" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F29" s="6">
         <v>5.0</v>
@@ -1681,7 +1681,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F31" s="6">
         <v>5.0</v>
@@ -1786,7 +1786,7 @@
         <v>27</v>
       </c>
       <c r="E34" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F34" s="6">
         <v>5.0</v>
@@ -1856,7 +1856,7 @@
         <v>27</v>
       </c>
       <c r="E36" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F36" s="6">
         <v>5.0</v>
@@ -1961,7 +1961,7 @@
         <v>27</v>
       </c>
       <c r="E39" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F39" s="6">
         <v>5.0</v>
@@ -2031,7 +2031,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F41" s="6">
         <v>5.0</v>
@@ -2136,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="E44" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F44" s="6">
         <v>5.0</v>
@@ -2206,7 +2206,7 @@
         <v>27</v>
       </c>
       <c r="E46" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F46" s="6">
         <v>5.0</v>
@@ -2311,7 +2311,7 @@
         <v>27</v>
       </c>
       <c r="E49" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F49" s="6">
         <v>5.0</v>
@@ -2381,7 +2381,7 @@
         <v>27</v>
       </c>
       <c r="E51" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F51" s="6">
         <v>5.0</v>
@@ -2486,7 +2486,7 @@
         <v>27</v>
       </c>
       <c r="E54" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F54" s="6">
         <v>5.0</v>
@@ -2556,7 +2556,7 @@
         <v>27</v>
       </c>
       <c r="E56" s="5">
-        <v>0.75</v>
+        <v>0.55</v>
       </c>
       <c r="F56" s="6">
         <v>5.0</v>
@@ -2731,7 +2731,7 @@
         <v>27</v>
       </c>
       <c r="E61" s="5">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F61" s="6">
         <v>5.0</v>

</xml_diff>